<commit_message>
moved system definition in a separate module
</commit_message>
<xml_diff>
--- a/data/Alloy_Sorting.xlsx
+++ b/data/Alloy_Sorting.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romainb\Documents\6. Papers\6. Dynamic MFA Al in Passenger cars\Dynamic-MFA-Al-in-Passenger-Cars\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\home.ansatt.ntnu.no\romainb\Documents\6. Papers\6. Dynamic MFA Al in Passenger cars\Dynamic-MFA-Al-in-Passenger-Cars\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7337F6B6-5701-432E-A59C-5837CA95A983}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86ECEC29-C6C8-4CAF-93D9-53764CBE6AA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{66C38FE6-7F1B-4F07-9DE9-E34F60D40B66}"/>
   </bookViews>
@@ -660,16 +660,16 @@
       <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -687,7 +687,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -707,7 +707,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
@@ -725,7 +725,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
@@ -747,7 +747,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>13</v>
       </c>
@@ -769,7 +769,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>16</v>
       </c>
@@ -791,7 +791,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>19</v>
       </c>
@@ -811,7 +811,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -829,7 +829,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
@@ -847,7 +847,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>28</v>
       </c>
@@ -863,7 +863,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
@@ -881,7 +881,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>32</v>
       </c>
@@ -899,7 +899,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>34</v>
       </c>
@@ -917,7 +917,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>36</v>
       </c>
@@ -935,7 +935,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>39</v>
       </c>
@@ -953,7 +953,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>41</v>
       </c>
@@ -965,7 +965,7 @@
       <c r="G16" s="4"/>
       <c r="H16" s="3"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>41</v>
       </c>
@@ -977,7 +977,7 @@
       <c r="G17" s="4"/>
       <c r="H17" s="3"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>41</v>
       </c>
@@ -989,7 +989,7 @@
       <c r="G18" s="4"/>
       <c r="H18" s="3"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>41</v>
       </c>
@@ -1001,7 +1001,7 @@
       <c r="G19" s="4"/>
       <c r="H19" s="3"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>41</v>
       </c>
@@ -1013,7 +1013,7 @@
       <c r="G20" s="4"/>
       <c r="H20" s="3"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>42</v>
       </c>
@@ -1039,7 +1039,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>46</v>
       </c>
@@ -1063,7 +1063,7 @@
       </c>
       <c r="H22" s="3"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>56</v>
       </c>
@@ -1089,7 +1089,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E24" s="4" t="s">
         <v>2</v>
       </c>
@@ -1103,7 +1103,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
@@ -1114,7 +1114,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="4" t="s">
@@ -1124,7 +1124,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
       <c r="G27" s="4" t="s">
@@ -1132,7 +1132,7 @@
       </c>
       <c r="H27" s="3"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1144,6 +1144,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1151,19 +1152,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F525485-5BF7-4B7F-9D80-F8AD30318E4F}">
   <dimension ref="A1:F152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="N133" sqref="M133:N133"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="J150" sqref="J150"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1180,7 +1181,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1900</v>
       </c>
@@ -1200,7 +1201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1901</v>
       </c>
@@ -1220,7 +1221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1902</v>
       </c>
@@ -1240,7 +1241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1903</v>
       </c>
@@ -1260,7 +1261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1904</v>
       </c>
@@ -1280,7 +1281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1905</v>
       </c>
@@ -1300,7 +1301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>1906</v>
       </c>
@@ -1320,7 +1321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1907</v>
       </c>
@@ -1340,7 +1341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1908</v>
       </c>
@@ -1360,7 +1361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>1909</v>
       </c>
@@ -1380,7 +1381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>1910</v>
       </c>
@@ -1400,7 +1401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>1911</v>
       </c>
@@ -1420,7 +1421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>1912</v>
       </c>
@@ -1440,7 +1441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>1913</v>
       </c>
@@ -1460,7 +1461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>1914</v>
       </c>
@@ -1480,7 +1481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>1915</v>
       </c>
@@ -1500,7 +1501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>1916</v>
       </c>
@@ -1520,7 +1521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>1917</v>
       </c>
@@ -1540,7 +1541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>1918</v>
       </c>
@@ -1560,7 +1561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>1919</v>
       </c>
@@ -1580,7 +1581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>1920</v>
       </c>
@@ -1600,7 +1601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>1921</v>
       </c>
@@ -1620,7 +1621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>1922</v>
       </c>
@@ -1640,7 +1641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>1923</v>
       </c>
@@ -1660,7 +1661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>1924</v>
       </c>
@@ -1680,7 +1681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>1925</v>
       </c>
@@ -1700,7 +1701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>1926</v>
       </c>
@@ -1720,7 +1721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>1927</v>
       </c>
@@ -1740,7 +1741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>1928</v>
       </c>
@@ -1760,7 +1761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>1929</v>
       </c>
@@ -1780,7 +1781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>1930</v>
       </c>
@@ -1800,7 +1801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>1931</v>
       </c>
@@ -1820,7 +1821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>1932</v>
       </c>
@@ -1840,7 +1841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>1933</v>
       </c>
@@ -1860,7 +1861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>1934</v>
       </c>
@@ -1880,7 +1881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>1935</v>
       </c>
@@ -1900,7 +1901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>1936</v>
       </c>
@@ -1920,7 +1921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>1937</v>
       </c>
@@ -1940,7 +1941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>1938</v>
       </c>
@@ -1960,7 +1961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>1939</v>
       </c>
@@ -1980,7 +1981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>1940</v>
       </c>
@@ -2000,7 +2001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>1941</v>
       </c>
@@ -2020,7 +2021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>1942</v>
       </c>
@@ -2040,7 +2041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>1943</v>
       </c>
@@ -2060,7 +2061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>1944</v>
       </c>
@@ -2080,7 +2081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>1945</v>
       </c>
@@ -2100,7 +2101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>1946</v>
       </c>
@@ -2120,7 +2121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>1947</v>
       </c>
@@ -2140,7 +2141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>1948</v>
       </c>
@@ -2160,7 +2161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>1949</v>
       </c>
@@ -2180,7 +2181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>1950</v>
       </c>
@@ -2200,7 +2201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>1951</v>
       </c>
@@ -2220,7 +2221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>1952</v>
       </c>
@@ -2240,7 +2241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>1953</v>
       </c>
@@ -2260,7 +2261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>1954</v>
       </c>
@@ -2280,7 +2281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>1955</v>
       </c>
@@ -2300,7 +2301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>1956</v>
       </c>
@@ -2320,7 +2321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>1957</v>
       </c>
@@ -2340,7 +2341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>1958</v>
       </c>
@@ -2360,7 +2361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>1959</v>
       </c>
@@ -2380,7 +2381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>1960</v>
       </c>
@@ -2400,7 +2401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>1961</v>
       </c>
@@ -2420,7 +2421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>1962</v>
       </c>
@@ -2440,7 +2441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>1963</v>
       </c>
@@ -2460,7 +2461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>1964</v>
       </c>
@@ -2480,7 +2481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>1965</v>
       </c>
@@ -2500,7 +2501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>1966</v>
       </c>
@@ -2520,7 +2521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>1967</v>
       </c>
@@ -2540,7 +2541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>1968</v>
       </c>
@@ -2560,7 +2561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>1969</v>
       </c>
@@ -2580,7 +2581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>1970</v>
       </c>
@@ -2600,7 +2601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>1971</v>
       </c>
@@ -2620,7 +2621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>1972</v>
       </c>
@@ -2640,7 +2641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>1973</v>
       </c>
@@ -2660,7 +2661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>1974</v>
       </c>
@@ -2680,7 +2681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>1975</v>
       </c>
@@ -2700,7 +2701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>1976</v>
       </c>
@@ -2720,7 +2721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>1977</v>
       </c>
@@ -2740,7 +2741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>1978</v>
       </c>
@@ -2760,7 +2761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>1979</v>
       </c>
@@ -2780,7 +2781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>1980</v>
       </c>
@@ -2800,7 +2801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>1981</v>
       </c>
@@ -2820,7 +2821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>1982</v>
       </c>
@@ -2840,7 +2841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>1983</v>
       </c>
@@ -2860,7 +2861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>1984</v>
       </c>
@@ -2880,7 +2881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>1985</v>
       </c>
@@ -2900,7 +2901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>1986</v>
       </c>
@@ -2920,7 +2921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>1987</v>
       </c>
@@ -2940,7 +2941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>1988</v>
       </c>
@@ -2960,7 +2961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>1989</v>
       </c>
@@ -2980,7 +2981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>1990</v>
       </c>
@@ -3000,7 +3001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>1991</v>
       </c>
@@ -3020,7 +3021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>1992</v>
       </c>
@@ -3040,7 +3041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>1993</v>
       </c>
@@ -3060,7 +3061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>1994</v>
       </c>
@@ -3080,7 +3081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>1995</v>
       </c>
@@ -3100,7 +3101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>1996</v>
       </c>
@@ -3120,7 +3121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>1997</v>
       </c>
@@ -3140,7 +3141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>1998</v>
       </c>
@@ -3160,7 +3161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>1999</v>
       </c>
@@ -3180,7 +3181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>2000</v>
       </c>
@@ -3200,7 +3201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>2001</v>
       </c>
@@ -3220,7 +3221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>2002</v>
       </c>
@@ -3240,7 +3241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>2003</v>
       </c>
@@ -3260,7 +3261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>2004</v>
       </c>
@@ -3280,7 +3281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>2005</v>
       </c>
@@ -3300,7 +3301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>2006</v>
       </c>
@@ -3320,7 +3321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>2007</v>
       </c>
@@ -3340,7 +3341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>2008</v>
       </c>
@@ -3360,7 +3361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>2009</v>
       </c>
@@ -3380,7 +3381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>2010</v>
       </c>
@@ -3400,7 +3401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>2011</v>
       </c>
@@ -3420,7 +3421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>2012</v>
       </c>
@@ -3440,7 +3441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>2013</v>
       </c>
@@ -3460,7 +3461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>2014</v>
       </c>
@@ -3480,7 +3481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>2015</v>
       </c>
@@ -3500,7 +3501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>2016</v>
       </c>
@@ -3520,7 +3521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>2017</v>
       </c>
@@ -3540,7 +3541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>2018</v>
       </c>
@@ -3560,7 +3561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>2019</v>
       </c>
@@ -3580,7 +3581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>2020</v>
       </c>
@@ -3600,752 +3601,753 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>2021</v>
       </c>
       <c r="B123" s="14">
         <f>B122+(B$152-B$122)/30</f>
-        <v>2.5000000000000001E-2</v>
+        <v>6.6666666666666671E-3</v>
       </c>
       <c r="C123" s="14">
         <f t="shared" ref="C123:F138" si="0">C122+(C$152-C$122)/30</f>
-        <v>2.5000000000000001E-2</v>
+        <v>6.6666666666666671E-3</v>
       </c>
       <c r="D123" s="14">
         <f t="shared" si="0"/>
-        <v>2.5000000000000001E-2</v>
+        <v>6.6666666666666671E-3</v>
       </c>
       <c r="E123" s="14">
         <f t="shared" si="0"/>
-        <v>2.5000000000000001E-2</v>
+        <v>6.6666666666666671E-3</v>
       </c>
       <c r="F123" s="14">
         <f t="shared" si="0"/>
-        <v>2.5000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+        <v>6.6666666666666671E-3</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>2022</v>
       </c>
       <c r="B124" s="14">
         <f t="shared" ref="B124:B151" si="1">B123+(B$152-B$122)/30</f>
-        <v>0.05</v>
+        <v>1.3333333333333334E-2</v>
       </c>
       <c r="C124" s="14">
         <f t="shared" si="0"/>
-        <v>0.05</v>
+        <v>1.3333333333333334E-2</v>
       </c>
       <c r="D124" s="14">
         <f t="shared" si="0"/>
-        <v>0.05</v>
+        <v>1.3333333333333334E-2</v>
       </c>
       <c r="E124" s="14">
         <f t="shared" si="0"/>
-        <v>0.05</v>
+        <v>1.3333333333333334E-2</v>
       </c>
       <c r="F124" s="14">
         <f t="shared" si="0"/>
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+        <v>1.3333333333333334E-2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>2023</v>
       </c>
       <c r="B125" s="14">
         <f t="shared" si="1"/>
-        <v>7.5000000000000011E-2</v>
+        <v>0.02</v>
       </c>
       <c r="C125" s="14">
         <f t="shared" si="0"/>
-        <v>7.5000000000000011E-2</v>
+        <v>0.02</v>
       </c>
       <c r="D125" s="14">
         <f t="shared" si="0"/>
-        <v>7.5000000000000011E-2</v>
+        <v>0.02</v>
       </c>
       <c r="E125" s="14">
         <f t="shared" si="0"/>
-        <v>7.5000000000000011E-2</v>
+        <v>0.02</v>
       </c>
       <c r="F125" s="14">
         <f t="shared" si="0"/>
-        <v>7.5000000000000011E-2</v>
-      </c>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>2024</v>
       </c>
       <c r="B126" s="14">
         <f t="shared" si="1"/>
-        <v>0.1</v>
+        <v>2.6666666666666668E-2</v>
       </c>
       <c r="C126" s="14">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>2.6666666666666668E-2</v>
       </c>
       <c r="D126" s="14">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>2.6666666666666668E-2</v>
       </c>
       <c r="E126" s="14">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>2.6666666666666668E-2</v>
       </c>
       <c r="F126" s="14">
         <f t="shared" si="0"/>
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+        <v>2.6666666666666668E-2</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>2025</v>
       </c>
       <c r="B127" s="14">
         <f t="shared" si="1"/>
-        <v>0.125</v>
+        <v>3.3333333333333333E-2</v>
       </c>
       <c r="C127" s="14">
         <f t="shared" si="0"/>
-        <v>0.125</v>
+        <v>3.3333333333333333E-2</v>
       </c>
       <c r="D127" s="14">
         <f t="shared" si="0"/>
-        <v>0.125</v>
+        <v>3.3333333333333333E-2</v>
       </c>
       <c r="E127" s="14">
         <f t="shared" si="0"/>
-        <v>0.125</v>
+        <v>3.3333333333333333E-2</v>
       </c>
       <c r="F127" s="14">
         <f t="shared" si="0"/>
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+        <v>3.3333333333333333E-2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>2026</v>
       </c>
       <c r="B128" s="14">
         <f t="shared" si="1"/>
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
       <c r="C128" s="14">
         <f t="shared" si="0"/>
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
       <c r="D128" s="14">
         <f t="shared" si="0"/>
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
       <c r="E128" s="14">
         <f t="shared" si="0"/>
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
       <c r="F128" s="14">
         <f t="shared" si="0"/>
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>2027</v>
       </c>
       <c r="B129" s="14">
         <f t="shared" si="1"/>
-        <v>0.17499999999999999</v>
+        <v>4.6666666666666669E-2</v>
       </c>
       <c r="C129" s="14">
         <f t="shared" si="0"/>
-        <v>0.17499999999999999</v>
+        <v>4.6666666666666669E-2</v>
       </c>
       <c r="D129" s="14">
         <f t="shared" si="0"/>
-        <v>0.17499999999999999</v>
+        <v>4.6666666666666669E-2</v>
       </c>
       <c r="E129" s="14">
         <f t="shared" si="0"/>
-        <v>0.17499999999999999</v>
+        <v>4.6666666666666669E-2</v>
       </c>
       <c r="F129" s="14">
         <f t="shared" si="0"/>
-        <v>0.17499999999999999</v>
-      </c>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
+        <v>4.6666666666666669E-2</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>2028</v>
       </c>
       <c r="B130" s="14">
         <f t="shared" si="1"/>
-        <v>0.19999999999999998</v>
+        <v>5.3333333333333337E-2</v>
       </c>
       <c r="C130" s="14">
         <f t="shared" si="0"/>
-        <v>0.19999999999999998</v>
+        <v>5.3333333333333337E-2</v>
       </c>
       <c r="D130" s="14">
         <f t="shared" si="0"/>
-        <v>0.19999999999999998</v>
+        <v>5.3333333333333337E-2</v>
       </c>
       <c r="E130" s="14">
         <f t="shared" si="0"/>
-        <v>0.19999999999999998</v>
+        <v>5.3333333333333337E-2</v>
       </c>
       <c r="F130" s="14">
         <f t="shared" si="0"/>
-        <v>0.19999999999999998</v>
-      </c>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
+        <v>5.3333333333333337E-2</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>2029</v>
       </c>
       <c r="B131" s="14">
         <f t="shared" si="1"/>
-        <v>0.22499999999999998</v>
+        <v>6.0000000000000005E-2</v>
       </c>
       <c r="C131" s="14">
         <f t="shared" si="0"/>
-        <v>0.22499999999999998</v>
+        <v>6.0000000000000005E-2</v>
       </c>
       <c r="D131" s="14">
         <f t="shared" si="0"/>
-        <v>0.22499999999999998</v>
+        <v>6.0000000000000005E-2</v>
       </c>
       <c r="E131" s="14">
         <f t="shared" si="0"/>
-        <v>0.22499999999999998</v>
+        <v>6.0000000000000005E-2</v>
       </c>
       <c r="F131" s="14">
         <f t="shared" si="0"/>
-        <v>0.22499999999999998</v>
-      </c>
-    </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
+        <v>6.0000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>2030</v>
       </c>
       <c r="B132" s="14">
         <f t="shared" si="1"/>
-        <v>0.24999999999999997</v>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="C132" s="14">
         <f t="shared" si="0"/>
-        <v>0.24999999999999997</v>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="D132" s="14">
         <f t="shared" si="0"/>
-        <v>0.24999999999999997</v>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="E132" s="14">
         <f t="shared" si="0"/>
-        <v>0.24999999999999997</v>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="F132" s="14">
         <f t="shared" si="0"/>
-        <v>0.24999999999999997</v>
-      </c>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
+        <v>6.6666666666666666E-2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>2031</v>
       </c>
       <c r="B133" s="14">
         <f t="shared" si="1"/>
-        <v>0.27499999999999997</v>
+        <v>7.3333333333333334E-2</v>
       </c>
       <c r="C133" s="14">
         <f t="shared" si="0"/>
-        <v>0.27499999999999997</v>
+        <v>7.3333333333333334E-2</v>
       </c>
       <c r="D133" s="14">
         <f t="shared" si="0"/>
-        <v>0.27499999999999997</v>
+        <v>7.3333333333333334E-2</v>
       </c>
       <c r="E133" s="14">
         <f t="shared" si="0"/>
-        <v>0.27499999999999997</v>
+        <v>7.3333333333333334E-2</v>
       </c>
       <c r="F133" s="14">
         <f t="shared" si="0"/>
-        <v>0.27499999999999997</v>
-      </c>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
+        <v>7.3333333333333334E-2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>2032</v>
       </c>
       <c r="B134" s="14">
         <f t="shared" si="1"/>
-        <v>0.3</v>
+        <v>0.08</v>
       </c>
       <c r="C134" s="14">
         <f t="shared" si="0"/>
-        <v>0.3</v>
+        <v>0.08</v>
       </c>
       <c r="D134" s="14">
         <f t="shared" si="0"/>
-        <v>0.3</v>
+        <v>0.08</v>
       </c>
       <c r="E134" s="14">
         <f t="shared" si="0"/>
-        <v>0.3</v>
+        <v>0.08</v>
       </c>
       <c r="F134" s="14">
         <f t="shared" si="0"/>
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>2033</v>
       </c>
       <c r="B135" s="14">
         <f t="shared" si="1"/>
-        <v>0.32500000000000001</v>
+        <v>8.666666666666667E-2</v>
       </c>
       <c r="C135" s="14">
         <f t="shared" si="0"/>
-        <v>0.32500000000000001</v>
+        <v>8.666666666666667E-2</v>
       </c>
       <c r="D135" s="14">
         <f t="shared" si="0"/>
-        <v>0.32500000000000001</v>
+        <v>8.666666666666667E-2</v>
       </c>
       <c r="E135" s="14">
         <f t="shared" si="0"/>
-        <v>0.32500000000000001</v>
+        <v>8.666666666666667E-2</v>
       </c>
       <c r="F135" s="14">
         <f t="shared" si="0"/>
-        <v>0.32500000000000001</v>
-      </c>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
+        <v>8.666666666666667E-2</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>2034</v>
       </c>
       <c r="B136" s="14">
         <f t="shared" si="1"/>
-        <v>0.35000000000000003</v>
+        <v>9.3333333333333338E-2</v>
       </c>
       <c r="C136" s="14">
         <f t="shared" si="0"/>
-        <v>0.35000000000000003</v>
+        <v>9.3333333333333338E-2</v>
       </c>
       <c r="D136" s="14">
         <f t="shared" si="0"/>
-        <v>0.35000000000000003</v>
+        <v>9.3333333333333338E-2</v>
       </c>
       <c r="E136" s="14">
         <f t="shared" si="0"/>
-        <v>0.35000000000000003</v>
+        <v>9.3333333333333338E-2</v>
       </c>
       <c r="F136" s="14">
         <f t="shared" si="0"/>
-        <v>0.35000000000000003</v>
-      </c>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
+        <v>9.3333333333333338E-2</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>2035</v>
       </c>
       <c r="B137" s="14">
         <f t="shared" si="1"/>
-        <v>0.37500000000000006</v>
+        <v>0.1</v>
       </c>
       <c r="C137" s="14">
         <f t="shared" si="0"/>
-        <v>0.37500000000000006</v>
+        <v>0.1</v>
       </c>
       <c r="D137" s="14">
         <f t="shared" si="0"/>
-        <v>0.37500000000000006</v>
+        <v>0.1</v>
       </c>
       <c r="E137" s="14">
         <f t="shared" si="0"/>
-        <v>0.37500000000000006</v>
+        <v>0.1</v>
       </c>
       <c r="F137" s="14">
         <f t="shared" si="0"/>
-        <v>0.37500000000000006</v>
-      </c>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>2036</v>
       </c>
       <c r="B138" s="14">
         <f t="shared" si="1"/>
-        <v>0.40000000000000008</v>
+        <v>0.10666666666666667</v>
       </c>
       <c r="C138" s="14">
         <f t="shared" si="0"/>
-        <v>0.40000000000000008</v>
+        <v>0.10666666666666667</v>
       </c>
       <c r="D138" s="14">
         <f t="shared" si="0"/>
-        <v>0.40000000000000008</v>
+        <v>0.10666666666666667</v>
       </c>
       <c r="E138" s="14">
         <f t="shared" si="0"/>
-        <v>0.40000000000000008</v>
+        <v>0.10666666666666667</v>
       </c>
       <c r="F138" s="14">
         <f t="shared" si="0"/>
-        <v>0.40000000000000008</v>
-      </c>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.10666666666666667</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>2037</v>
       </c>
       <c r="B139" s="14">
         <f t="shared" si="1"/>
-        <v>0.4250000000000001</v>
+        <v>0.11333333333333334</v>
       </c>
       <c r="C139" s="14">
         <f t="shared" ref="C139:C151" si="2">C138+(C$152-C$122)/30</f>
-        <v>0.4250000000000001</v>
+        <v>0.11333333333333334</v>
       </c>
       <c r="D139" s="14">
         <f t="shared" ref="D139:D151" si="3">D138+(D$152-D$122)/30</f>
-        <v>0.4250000000000001</v>
+        <v>0.11333333333333334</v>
       </c>
       <c r="E139" s="14">
         <f t="shared" ref="E139:E151" si="4">E138+(E$152-E$122)/30</f>
-        <v>0.4250000000000001</v>
+        <v>0.11333333333333334</v>
       </c>
       <c r="F139" s="14">
         <f t="shared" ref="F139:F151" si="5">F138+(F$152-F$122)/30</f>
-        <v>0.4250000000000001</v>
-      </c>
-    </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.11333333333333334</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>2038</v>
       </c>
       <c r="B140" s="14">
         <f t="shared" si="1"/>
-        <v>0.45000000000000012</v>
+        <v>0.12000000000000001</v>
       </c>
       <c r="C140" s="14">
         <f t="shared" si="2"/>
-        <v>0.45000000000000012</v>
+        <v>0.12000000000000001</v>
       </c>
       <c r="D140" s="14">
         <f t="shared" si="3"/>
-        <v>0.45000000000000012</v>
+        <v>0.12000000000000001</v>
       </c>
       <c r="E140" s="14">
         <f t="shared" si="4"/>
-        <v>0.45000000000000012</v>
+        <v>0.12000000000000001</v>
       </c>
       <c r="F140" s="14">
         <f t="shared" si="5"/>
-        <v>0.45000000000000012</v>
-      </c>
-    </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.12000000000000001</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>2039</v>
       </c>
       <c r="B141" s="14">
         <f t="shared" si="1"/>
-        <v>0.47500000000000014</v>
+        <v>0.12666666666666668</v>
       </c>
       <c r="C141" s="14">
         <f t="shared" si="2"/>
-        <v>0.47500000000000014</v>
+        <v>0.12666666666666668</v>
       </c>
       <c r="D141" s="14">
         <f t="shared" si="3"/>
-        <v>0.47500000000000014</v>
+        <v>0.12666666666666668</v>
       </c>
       <c r="E141" s="14">
         <f t="shared" si="4"/>
-        <v>0.47500000000000014</v>
+        <v>0.12666666666666668</v>
       </c>
       <c r="F141" s="14">
         <f t="shared" si="5"/>
-        <v>0.47500000000000014</v>
-      </c>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.12666666666666668</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>2040</v>
       </c>
       <c r="B142" s="14">
         <f t="shared" si="1"/>
-        <v>0.50000000000000011</v>
+        <v>0.13333333333333333</v>
       </c>
       <c r="C142" s="14">
         <f t="shared" si="2"/>
-        <v>0.50000000000000011</v>
+        <v>0.13333333333333333</v>
       </c>
       <c r="D142" s="14">
         <f t="shared" si="3"/>
-        <v>0.50000000000000011</v>
+        <v>0.13333333333333333</v>
       </c>
       <c r="E142" s="14">
         <f t="shared" si="4"/>
-        <v>0.50000000000000011</v>
+        <v>0.13333333333333333</v>
       </c>
       <c r="F142" s="14">
         <f t="shared" si="5"/>
-        <v>0.50000000000000011</v>
-      </c>
-    </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.13333333333333333</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>2041</v>
       </c>
       <c r="B143" s="14">
         <f t="shared" si="1"/>
-        <v>0.52500000000000013</v>
+        <v>0.13999999999999999</v>
       </c>
       <c r="C143" s="14">
         <f t="shared" si="2"/>
-        <v>0.52500000000000013</v>
+        <v>0.13999999999999999</v>
       </c>
       <c r="D143" s="14">
         <f t="shared" si="3"/>
-        <v>0.52500000000000013</v>
+        <v>0.13999999999999999</v>
       </c>
       <c r="E143" s="14">
         <f t="shared" si="4"/>
-        <v>0.52500000000000013</v>
+        <v>0.13999999999999999</v>
       </c>
       <c r="F143" s="14">
         <f t="shared" si="5"/>
-        <v>0.52500000000000013</v>
-      </c>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.13999999999999999</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>2042</v>
       </c>
       <c r="B144" s="14">
         <f t="shared" si="1"/>
-        <v>0.55000000000000016</v>
+        <v>0.14666666666666664</v>
       </c>
       <c r="C144" s="14">
         <f t="shared" si="2"/>
-        <v>0.55000000000000016</v>
+        <v>0.14666666666666664</v>
       </c>
       <c r="D144" s="14">
         <f t="shared" si="3"/>
-        <v>0.55000000000000016</v>
+        <v>0.14666666666666664</v>
       </c>
       <c r="E144" s="14">
         <f t="shared" si="4"/>
-        <v>0.55000000000000016</v>
+        <v>0.14666666666666664</v>
       </c>
       <c r="F144" s="14">
         <f t="shared" si="5"/>
-        <v>0.55000000000000016</v>
-      </c>
-    </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.14666666666666664</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>2043</v>
       </c>
       <c r="B145" s="14">
         <f t="shared" si="1"/>
-        <v>0.57500000000000018</v>
+        <v>0.15333333333333329</v>
       </c>
       <c r="C145" s="14">
         <f t="shared" si="2"/>
-        <v>0.57500000000000018</v>
+        <v>0.15333333333333329</v>
       </c>
       <c r="D145" s="14">
         <f t="shared" si="3"/>
-        <v>0.57500000000000018</v>
+        <v>0.15333333333333329</v>
       </c>
       <c r="E145" s="14">
         <f t="shared" si="4"/>
-        <v>0.57500000000000018</v>
+        <v>0.15333333333333329</v>
       </c>
       <c r="F145" s="14">
         <f t="shared" si="5"/>
-        <v>0.57500000000000018</v>
-      </c>
-    </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.15333333333333329</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>2044</v>
       </c>
       <c r="B146" s="14">
         <f t="shared" si="1"/>
-        <v>0.6000000000000002</v>
+        <v>0.15999999999999995</v>
       </c>
       <c r="C146" s="14">
         <f t="shared" si="2"/>
-        <v>0.6000000000000002</v>
+        <v>0.15999999999999995</v>
       </c>
       <c r="D146" s="14">
         <f t="shared" si="3"/>
-        <v>0.6000000000000002</v>
+        <v>0.15999999999999995</v>
       </c>
       <c r="E146" s="14">
         <f t="shared" si="4"/>
-        <v>0.6000000000000002</v>
+        <v>0.15999999999999995</v>
       </c>
       <c r="F146" s="14">
         <f t="shared" si="5"/>
-        <v>0.6000000000000002</v>
-      </c>
-    </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.15999999999999995</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>2045</v>
       </c>
       <c r="B147" s="14">
         <f t="shared" si="1"/>
-        <v>0.62500000000000022</v>
+        <v>0.1666666666666666</v>
       </c>
       <c r="C147" s="14">
         <f t="shared" si="2"/>
-        <v>0.62500000000000022</v>
+        <v>0.1666666666666666</v>
       </c>
       <c r="D147" s="14">
         <f t="shared" si="3"/>
-        <v>0.62500000000000022</v>
+        <v>0.1666666666666666</v>
       </c>
       <c r="E147" s="14">
         <f t="shared" si="4"/>
-        <v>0.62500000000000022</v>
+        <v>0.1666666666666666</v>
       </c>
       <c r="F147" s="14">
         <f t="shared" si="5"/>
-        <v>0.62500000000000022</v>
-      </c>
-    </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.1666666666666666</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>2046</v>
       </c>
       <c r="B148" s="14">
         <f t="shared" si="1"/>
-        <v>0.65000000000000024</v>
+        <v>0.17333333333333326</v>
       </c>
       <c r="C148" s="14">
         <f t="shared" si="2"/>
-        <v>0.65000000000000024</v>
+        <v>0.17333333333333326</v>
       </c>
       <c r="D148" s="14">
         <f t="shared" si="3"/>
-        <v>0.65000000000000024</v>
+        <v>0.17333333333333326</v>
       </c>
       <c r="E148" s="14">
         <f t="shared" si="4"/>
-        <v>0.65000000000000024</v>
+        <v>0.17333333333333326</v>
       </c>
       <c r="F148" s="14">
         <f t="shared" si="5"/>
-        <v>0.65000000000000024</v>
-      </c>
-    </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.17333333333333326</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>2047</v>
       </c>
       <c r="B149" s="14">
         <f t="shared" si="1"/>
-        <v>0.67500000000000027</v>
+        <v>0.17999999999999991</v>
       </c>
       <c r="C149" s="14">
         <f t="shared" si="2"/>
-        <v>0.67500000000000027</v>
+        <v>0.17999999999999991</v>
       </c>
       <c r="D149" s="14">
         <f t="shared" si="3"/>
-        <v>0.67500000000000027</v>
+        <v>0.17999999999999991</v>
       </c>
       <c r="E149" s="14">
         <f t="shared" si="4"/>
-        <v>0.67500000000000027</v>
+        <v>0.17999999999999991</v>
       </c>
       <c r="F149" s="14">
         <f t="shared" si="5"/>
-        <v>0.67500000000000027</v>
-      </c>
-    </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.17999999999999991</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>2048</v>
       </c>
       <c r="B150" s="14">
         <f t="shared" si="1"/>
-        <v>0.70000000000000029</v>
+        <v>0.18666666666666656</v>
       </c>
       <c r="C150" s="14">
         <f t="shared" si="2"/>
-        <v>0.70000000000000029</v>
+        <v>0.18666666666666656</v>
       </c>
       <c r="D150" s="14">
         <f t="shared" si="3"/>
-        <v>0.70000000000000029</v>
+        <v>0.18666666666666656</v>
       </c>
       <c r="E150" s="14">
         <f t="shared" si="4"/>
-        <v>0.70000000000000029</v>
+        <v>0.18666666666666656</v>
       </c>
       <c r="F150" s="14">
         <f t="shared" si="5"/>
-        <v>0.70000000000000029</v>
-      </c>
-    </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.18666666666666656</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>2049</v>
       </c>
       <c r="B151" s="14">
         <f t="shared" si="1"/>
-        <v>0.72500000000000031</v>
+        <v>0.19333333333333322</v>
       </c>
       <c r="C151" s="14">
         <f t="shared" si="2"/>
-        <v>0.72500000000000031</v>
+        <v>0.19333333333333322</v>
       </c>
       <c r="D151" s="14">
         <f t="shared" si="3"/>
-        <v>0.72500000000000031</v>
+        <v>0.19333333333333322</v>
       </c>
       <c r="E151" s="14">
         <f t="shared" si="4"/>
-        <v>0.72500000000000031</v>
+        <v>0.19333333333333322</v>
       </c>
       <c r="F151" s="14">
         <f t="shared" si="5"/>
-        <v>0.72500000000000031</v>
-      </c>
-    </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.19333333333333322</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>2050</v>
       </c>
       <c r="B152" s="14">
-        <v>0.75</v>
+        <v>0.2</v>
       </c>
       <c r="C152" s="14">
-        <v>0.75</v>
+        <v>0.2</v>
       </c>
       <c r="D152" s="14">
-        <v>0.75</v>
+        <v>0.2</v>
       </c>
       <c r="E152" s="14">
-        <v>0.75</v>
+        <v>0.2</v>
       </c>
       <c r="F152" s="14">
-        <v>0.75</v>
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Corrections for alloy sorting
</commit_message>
<xml_diff>
--- a/data/Alloy_Sorting.xlsx
+++ b/data/Alloy_Sorting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\home.ansatt.ntnu.no\romainb\Documents\6. Papers\6. Dynamic MFA Al in Passenger cars\Dynamic-MFA-Al-in-Passenger-Cars\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C43A61D-728A-48E6-BD94-B689752DC18A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D102D0-7503-4D7C-A41C-5B9588E58ADE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{66C38FE6-7F1B-4F07-9DE9-E34F60D40B66}"/>
   </bookViews>
@@ -676,7 +676,7 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D32" sqref="D32:E32"/>
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1177,8 +1177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F525485-5BF7-4B7F-9D80-F8AD30318E4F}">
   <dimension ref="A1:G454"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A415" workbookViewId="0">
-      <selection activeCell="N444" sqref="N444"/>
+    <sheetView tabSelected="1" topLeftCell="A269" workbookViewId="0">
+      <selection activeCell="J289" sqref="J289"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7616,23 +7616,23 @@
         <v>2021</v>
       </c>
       <c r="C274" s="14">
-        <f>C273+(C$303-C$273)/30</f>
+        <f t="shared" ref="C274:C301" si="6">C273+(C$303-C$273)/30</f>
         <v>2.6666666666666668E-2</v>
       </c>
       <c r="D274" s="14">
-        <f t="shared" ref="D274:G274" si="6">D273+(D$303-D$273)/30</f>
+        <f t="shared" ref="D274:D301" si="7">D273+(D$303-D$273)/30</f>
         <v>2.6666666666666668E-2</v>
       </c>
       <c r="E274" s="14">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="E274:E301" si="8">E273+(E$303-E$273)/30</f>
         <v>1.6666666666666666E-2</v>
       </c>
       <c r="F274" s="14">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="F274:F301" si="9">F273+(F$303-F$273)/30</f>
         <v>2.6666666666666668E-2</v>
       </c>
       <c r="G274" s="14">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="G274:G301" si="10">G273+(G$303-G$273)/30</f>
         <v>1.6666666666666666E-2</v>
       </c>
     </row>
@@ -7644,24 +7644,24 @@
         <v>2022</v>
       </c>
       <c r="C275" s="14">
-        <f t="shared" ref="C275:G290" si="7">C274+(C$152-C$122)/30</f>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="6"/>
+        <v>5.3333333333333337E-2</v>
       </c>
       <c r="D275" s="14">
         <f t="shared" si="7"/>
-        <v>2.6666666666666668E-2</v>
+        <v>5.3333333333333337E-2</v>
       </c>
       <c r="E275" s="14">
-        <f t="shared" si="7"/>
-        <v>1.6666666666666666E-2</v>
+        <f t="shared" si="8"/>
+        <v>3.3333333333333333E-2</v>
       </c>
       <c r="F275" s="14">
-        <f t="shared" si="7"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="9"/>
+        <v>5.3333333333333337E-2</v>
       </c>
       <c r="G275" s="14">
-        <f t="shared" si="7"/>
-        <v>1.6666666666666666E-2</v>
+        <f t="shared" si="10"/>
+        <v>3.3333333333333333E-2</v>
       </c>
     </row>
     <row r="276" spans="1:7" x14ac:dyDescent="0.3">
@@ -7672,24 +7672,24 @@
         <v>2023</v>
       </c>
       <c r="C276" s="14">
-        <f t="shared" si="7"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="6"/>
+        <v>0.08</v>
       </c>
       <c r="D276" s="14">
         <f t="shared" si="7"/>
-        <v>2.6666666666666668E-2</v>
+        <v>0.08</v>
       </c>
       <c r="E276" s="14">
-        <f t="shared" si="7"/>
-        <v>1.6666666666666666E-2</v>
+        <f t="shared" si="8"/>
+        <v>0.05</v>
       </c>
       <c r="F276" s="14">
-        <f t="shared" si="7"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="9"/>
+        <v>0.08</v>
       </c>
       <c r="G276" s="14">
-        <f t="shared" si="7"/>
-        <v>1.6666666666666666E-2</v>
+        <f t="shared" si="10"/>
+        <v>0.05</v>
       </c>
     </row>
     <row r="277" spans="1:7" x14ac:dyDescent="0.3">
@@ -7700,24 +7700,24 @@
         <v>2024</v>
       </c>
       <c r="C277" s="14">
-        <f t="shared" si="7"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="6"/>
+        <v>0.10666666666666667</v>
       </c>
       <c r="D277" s="14">
         <f t="shared" si="7"/>
-        <v>2.6666666666666668E-2</v>
+        <v>0.10666666666666667</v>
       </c>
       <c r="E277" s="14">
-        <f t="shared" si="7"/>
-        <v>1.6666666666666666E-2</v>
+        <f t="shared" si="8"/>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="F277" s="14">
-        <f t="shared" si="7"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="9"/>
+        <v>0.10666666666666667</v>
       </c>
       <c r="G277" s="14">
-        <f t="shared" si="7"/>
-        <v>1.6666666666666666E-2</v>
+        <f t="shared" si="10"/>
+        <v>6.6666666666666666E-2</v>
       </c>
     </row>
     <row r="278" spans="1:7" x14ac:dyDescent="0.3">
@@ -7728,24 +7728,24 @@
         <v>2025</v>
       </c>
       <c r="C278" s="14">
-        <f t="shared" si="7"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="6"/>
+        <v>0.13333333333333333</v>
       </c>
       <c r="D278" s="14">
         <f t="shared" si="7"/>
-        <v>2.6666666666666668E-2</v>
+        <v>0.13333333333333333</v>
       </c>
       <c r="E278" s="14">
-        <f t="shared" si="7"/>
-        <v>1.6666666666666666E-2</v>
+        <f t="shared" si="8"/>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="F278" s="14">
-        <f t="shared" si="7"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="9"/>
+        <v>0.13333333333333333</v>
       </c>
       <c r="G278" s="14">
-        <f t="shared" si="7"/>
-        <v>1.6666666666666666E-2</v>
+        <f t="shared" si="10"/>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="279" spans="1:7" x14ac:dyDescent="0.3">
@@ -7756,24 +7756,24 @@
         <v>2026</v>
       </c>
       <c r="C279" s="14">
-        <f t="shared" si="7"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="6"/>
+        <v>0.16</v>
       </c>
       <c r="D279" s="14">
         <f t="shared" si="7"/>
-        <v>2.6666666666666668E-2</v>
+        <v>0.16</v>
       </c>
       <c r="E279" s="14">
-        <f t="shared" si="7"/>
-        <v>1.6666666666666666E-2</v>
+        <f t="shared" si="8"/>
+        <v>9.9999999999999992E-2</v>
       </c>
       <c r="F279" s="14">
-        <f t="shared" si="7"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="9"/>
+        <v>0.16</v>
       </c>
       <c r="G279" s="14">
-        <f t="shared" si="7"/>
-        <v>1.6666666666666666E-2</v>
+        <f t="shared" si="10"/>
+        <v>9.9999999999999992E-2</v>
       </c>
     </row>
     <row r="280" spans="1:7" x14ac:dyDescent="0.3">
@@ -7784,24 +7784,24 @@
         <v>2027</v>
       </c>
       <c r="C280" s="14">
-        <f t="shared" si="7"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="6"/>
+        <v>0.18666666666666668</v>
       </c>
       <c r="D280" s="14">
         <f t="shared" si="7"/>
-        <v>2.6666666666666668E-2</v>
+        <v>0.18666666666666668</v>
       </c>
       <c r="E280" s="14">
-        <f t="shared" si="7"/>
-        <v>1.6666666666666666E-2</v>
+        <f t="shared" si="8"/>
+        <v>0.11666666666666665</v>
       </c>
       <c r="F280" s="14">
-        <f t="shared" si="7"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="9"/>
+        <v>0.18666666666666668</v>
       </c>
       <c r="G280" s="14">
-        <f t="shared" si="7"/>
-        <v>1.6666666666666666E-2</v>
+        <f t="shared" si="10"/>
+        <v>0.11666666666666665</v>
       </c>
     </row>
     <row r="281" spans="1:7" x14ac:dyDescent="0.3">
@@ -7812,24 +7812,24 @@
         <v>2028</v>
       </c>
       <c r="C281" s="14">
-        <f t="shared" si="7"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="6"/>
+        <v>0.21333333333333335</v>
       </c>
       <c r="D281" s="14">
         <f t="shared" si="7"/>
-        <v>2.6666666666666668E-2</v>
+        <v>0.21333333333333335</v>
       </c>
       <c r="E281" s="14">
-        <f t="shared" si="7"/>
-        <v>1.6666666666666666E-2</v>
+        <f t="shared" si="8"/>
+        <v>0.13333333333333333</v>
       </c>
       <c r="F281" s="14">
-        <f t="shared" si="7"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="9"/>
+        <v>0.21333333333333335</v>
       </c>
       <c r="G281" s="14">
-        <f t="shared" si="7"/>
-        <v>1.6666666666666666E-2</v>
+        <f t="shared" si="10"/>
+        <v>0.13333333333333333</v>
       </c>
     </row>
     <row r="282" spans="1:7" x14ac:dyDescent="0.3">
@@ -7840,24 +7840,24 @@
         <v>2029</v>
       </c>
       <c r="C282" s="14">
-        <f t="shared" si="7"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="6"/>
+        <v>0.24000000000000002</v>
       </c>
       <c r="D282" s="14">
         <f t="shared" si="7"/>
-        <v>2.6666666666666668E-2</v>
+        <v>0.24000000000000002</v>
       </c>
       <c r="E282" s="14">
-        <f t="shared" si="7"/>
-        <v>1.6666666666666666E-2</v>
+        <f t="shared" si="8"/>
+        <v>0.15</v>
       </c>
       <c r="F282" s="14">
-        <f t="shared" si="7"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="9"/>
+        <v>0.24000000000000002</v>
       </c>
       <c r="G282" s="14">
-        <f t="shared" si="7"/>
-        <v>1.6666666666666666E-2</v>
+        <f t="shared" si="10"/>
+        <v>0.15</v>
       </c>
     </row>
     <row r="283" spans="1:7" x14ac:dyDescent="0.3">
@@ -7868,24 +7868,24 @@
         <v>2030</v>
       </c>
       <c r="C283" s="14">
-        <f t="shared" si="7"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="6"/>
+        <v>0.26666666666666666</v>
       </c>
       <c r="D283" s="14">
         <f t="shared" si="7"/>
-        <v>2.6666666666666668E-2</v>
+        <v>0.26666666666666666</v>
       </c>
       <c r="E283" s="14">
-        <f t="shared" si="7"/>
-        <v>1.6666666666666666E-2</v>
+        <f t="shared" si="8"/>
+        <v>0.16666666666666666</v>
       </c>
       <c r="F283" s="14">
-        <f t="shared" si="7"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="9"/>
+        <v>0.26666666666666666</v>
       </c>
       <c r="G283" s="14">
-        <f t="shared" si="7"/>
-        <v>1.6666666666666666E-2</v>
+        <f t="shared" si="10"/>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="284" spans="1:7" x14ac:dyDescent="0.3">
@@ -7896,24 +7896,24 @@
         <v>2031</v>
       </c>
       <c r="C284" s="14">
-        <f t="shared" si="7"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="6"/>
+        <v>0.29333333333333333</v>
       </c>
       <c r="D284" s="14">
         <f t="shared" si="7"/>
-        <v>2.6666666666666668E-2</v>
+        <v>0.29333333333333333</v>
       </c>
       <c r="E284" s="14">
-        <f t="shared" si="7"/>
-        <v>1.6666666666666666E-2</v>
+        <f t="shared" si="8"/>
+        <v>0.18333333333333332</v>
       </c>
       <c r="F284" s="14">
-        <f t="shared" si="7"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="9"/>
+        <v>0.29333333333333333</v>
       </c>
       <c r="G284" s="14">
-        <f t="shared" si="7"/>
-        <v>1.6666666666666666E-2</v>
+        <f t="shared" si="10"/>
+        <v>0.18333333333333332</v>
       </c>
     </row>
     <row r="285" spans="1:7" x14ac:dyDescent="0.3">
@@ -7924,24 +7924,24 @@
         <v>2032</v>
       </c>
       <c r="C285" s="14">
-        <f t="shared" si="7"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="6"/>
+        <v>0.32</v>
       </c>
       <c r="D285" s="14">
         <f t="shared" si="7"/>
-        <v>2.6666666666666668E-2</v>
+        <v>0.32</v>
       </c>
       <c r="E285" s="14">
-        <f t="shared" si="7"/>
-        <v>1.6666666666666666E-2</v>
+        <f t="shared" si="8"/>
+        <v>0.19999999999999998</v>
       </c>
       <c r="F285" s="14">
-        <f t="shared" si="7"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="9"/>
+        <v>0.32</v>
       </c>
       <c r="G285" s="14">
-        <f t="shared" si="7"/>
-        <v>1.6666666666666666E-2</v>
+        <f t="shared" si="10"/>
+        <v>0.19999999999999998</v>
       </c>
     </row>
     <row r="286" spans="1:7" x14ac:dyDescent="0.3">
@@ -7952,24 +7952,24 @@
         <v>2033</v>
       </c>
       <c r="C286" s="14">
-        <f t="shared" si="7"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="6"/>
+        <v>0.34666666666666668</v>
       </c>
       <c r="D286" s="14">
         <f t="shared" si="7"/>
-        <v>2.6666666666666668E-2</v>
+        <v>0.34666666666666668</v>
       </c>
       <c r="E286" s="14">
-        <f t="shared" si="7"/>
-        <v>1.6666666666666666E-2</v>
+        <f t="shared" si="8"/>
+        <v>0.21666666666666665</v>
       </c>
       <c r="F286" s="14">
-        <f t="shared" si="7"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="9"/>
+        <v>0.34666666666666668</v>
       </c>
       <c r="G286" s="14">
-        <f t="shared" si="7"/>
-        <v>1.6666666666666666E-2</v>
+        <f t="shared" si="10"/>
+        <v>0.21666666666666665</v>
       </c>
     </row>
     <row r="287" spans="1:7" x14ac:dyDescent="0.3">
@@ -7980,24 +7980,24 @@
         <v>2034</v>
       </c>
       <c r="C287" s="14">
-        <f t="shared" si="7"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="6"/>
+        <v>0.37333333333333335</v>
       </c>
       <c r="D287" s="14">
         <f t="shared" si="7"/>
-        <v>2.6666666666666668E-2</v>
+        <v>0.37333333333333335</v>
       </c>
       <c r="E287" s="14">
-        <f t="shared" si="7"/>
-        <v>1.6666666666666666E-2</v>
+        <f t="shared" si="8"/>
+        <v>0.23333333333333331</v>
       </c>
       <c r="F287" s="14">
-        <f t="shared" si="7"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="9"/>
+        <v>0.37333333333333335</v>
       </c>
       <c r="G287" s="14">
-        <f t="shared" si="7"/>
-        <v>1.6666666666666666E-2</v>
+        <f t="shared" si="10"/>
+        <v>0.23333333333333331</v>
       </c>
     </row>
     <row r="288" spans="1:7" x14ac:dyDescent="0.3">
@@ -8008,24 +8008,24 @@
         <v>2035</v>
       </c>
       <c r="C288" s="14">
-        <f t="shared" si="7"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="6"/>
+        <v>0.4</v>
       </c>
       <c r="D288" s="14">
         <f t="shared" si="7"/>
-        <v>2.6666666666666668E-2</v>
+        <v>0.4</v>
       </c>
       <c r="E288" s="14">
-        <f t="shared" si="7"/>
-        <v>1.6666666666666666E-2</v>
+        <f t="shared" si="8"/>
+        <v>0.24999999999999997</v>
       </c>
       <c r="F288" s="14">
-        <f t="shared" si="7"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="9"/>
+        <v>0.4</v>
       </c>
       <c r="G288" s="14">
-        <f t="shared" si="7"/>
-        <v>1.6666666666666666E-2</v>
+        <f t="shared" si="10"/>
+        <v>0.24999999999999997</v>
       </c>
     </row>
     <row r="289" spans="1:7" x14ac:dyDescent="0.3">
@@ -8036,24 +8036,24 @@
         <v>2036</v>
       </c>
       <c r="C289" s="14">
-        <f t="shared" si="7"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="6"/>
+        <v>0.42666666666666669</v>
       </c>
       <c r="D289" s="14">
         <f t="shared" si="7"/>
-        <v>2.6666666666666668E-2</v>
+        <v>0.42666666666666669</v>
       </c>
       <c r="E289" s="14">
-        <f t="shared" si="7"/>
-        <v>1.6666666666666666E-2</v>
+        <f t="shared" si="8"/>
+        <v>0.26666666666666666</v>
       </c>
       <c r="F289" s="14">
-        <f t="shared" si="7"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="9"/>
+        <v>0.42666666666666669</v>
       </c>
       <c r="G289" s="14">
-        <f t="shared" si="7"/>
-        <v>1.6666666666666666E-2</v>
+        <f t="shared" si="10"/>
+        <v>0.26666666666666666</v>
       </c>
     </row>
     <row r="290" spans="1:7" x14ac:dyDescent="0.3">
@@ -8064,24 +8064,24 @@
         <v>2037</v>
       </c>
       <c r="C290" s="14">
-        <f t="shared" si="7"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="6"/>
+        <v>0.45333333333333337</v>
       </c>
       <c r="D290" s="14">
         <f t="shared" si="7"/>
-        <v>2.6666666666666668E-2</v>
+        <v>0.45333333333333337</v>
       </c>
       <c r="E290" s="14">
-        <f t="shared" si="7"/>
-        <v>1.6666666666666666E-2</v>
+        <f t="shared" si="8"/>
+        <v>0.28333333333333333</v>
       </c>
       <c r="F290" s="14">
-        <f t="shared" si="7"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="9"/>
+        <v>0.45333333333333337</v>
       </c>
       <c r="G290" s="14">
-        <f t="shared" si="7"/>
-        <v>1.6666666666666666E-2</v>
+        <f t="shared" si="10"/>
+        <v>0.28333333333333333</v>
       </c>
     </row>
     <row r="291" spans="1:7" x14ac:dyDescent="0.3">
@@ -8092,24 +8092,24 @@
         <v>2038</v>
       </c>
       <c r="C291" s="14">
-        <f t="shared" ref="C291:G302" si="8">C290+(C$152-C$122)/30</f>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="6"/>
+        <v>0.48000000000000004</v>
       </c>
       <c r="D291" s="14">
-        <f t="shared" si="8"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="7"/>
+        <v>0.48000000000000004</v>
       </c>
       <c r="E291" s="14">
         <f t="shared" si="8"/>
-        <v>1.6666666666666666E-2</v>
+        <v>0.3</v>
       </c>
       <c r="F291" s="14">
-        <f t="shared" si="8"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="9"/>
+        <v>0.48000000000000004</v>
       </c>
       <c r="G291" s="14">
-        <f t="shared" si="8"/>
-        <v>1.6666666666666666E-2</v>
+        <f t="shared" si="10"/>
+        <v>0.3</v>
       </c>
     </row>
     <row r="292" spans="1:7" x14ac:dyDescent="0.3">
@@ -8120,24 +8120,24 @@
         <v>2039</v>
       </c>
       <c r="C292" s="14">
-        <f t="shared" si="8"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="6"/>
+        <v>0.50666666666666671</v>
       </c>
       <c r="D292" s="14">
-        <f t="shared" si="8"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="7"/>
+        <v>0.50666666666666671</v>
       </c>
       <c r="E292" s="14">
         <f t="shared" si="8"/>
-        <v>1.6666666666666666E-2</v>
+        <v>0.31666666666666665</v>
       </c>
       <c r="F292" s="14">
-        <f t="shared" si="8"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="9"/>
+        <v>0.50666666666666671</v>
       </c>
       <c r="G292" s="14">
-        <f t="shared" si="8"/>
-        <v>1.6666666666666666E-2</v>
+        <f t="shared" si="10"/>
+        <v>0.31666666666666665</v>
       </c>
     </row>
     <row r="293" spans="1:7" x14ac:dyDescent="0.3">
@@ -8148,24 +8148,24 @@
         <v>2040</v>
       </c>
       <c r="C293" s="14">
-        <f t="shared" si="8"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="6"/>
+        <v>0.53333333333333333</v>
       </c>
       <c r="D293" s="14">
-        <f t="shared" si="8"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="7"/>
+        <v>0.53333333333333333</v>
       </c>
       <c r="E293" s="14">
         <f t="shared" si="8"/>
-        <v>1.6666666666666666E-2</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="F293" s="14">
-        <f t="shared" si="8"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="9"/>
+        <v>0.53333333333333333</v>
       </c>
       <c r="G293" s="14">
-        <f t="shared" si="8"/>
-        <v>1.6666666666666666E-2</v>
+        <f t="shared" si="10"/>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="294" spans="1:7" x14ac:dyDescent="0.3">
@@ -8176,24 +8176,24 @@
         <v>2041</v>
       </c>
       <c r="C294" s="14">
-        <f t="shared" si="8"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="6"/>
+        <v>0.55999999999999994</v>
       </c>
       <c r="D294" s="14">
-        <f t="shared" si="8"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="7"/>
+        <v>0.55999999999999994</v>
       </c>
       <c r="E294" s="14">
         <f t="shared" si="8"/>
-        <v>1.6666666666666666E-2</v>
+        <v>0.35</v>
       </c>
       <c r="F294" s="14">
-        <f t="shared" si="8"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="9"/>
+        <v>0.55999999999999994</v>
       </c>
       <c r="G294" s="14">
-        <f t="shared" si="8"/>
-        <v>1.6666666666666666E-2</v>
+        <f t="shared" si="10"/>
+        <v>0.35</v>
       </c>
     </row>
     <row r="295" spans="1:7" x14ac:dyDescent="0.3">
@@ -8204,24 +8204,24 @@
         <v>2042</v>
       </c>
       <c r="C295" s="14">
-        <f t="shared" si="8"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="6"/>
+        <v>0.58666666666666656</v>
       </c>
       <c r="D295" s="14">
-        <f t="shared" si="8"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="7"/>
+        <v>0.58666666666666656</v>
       </c>
       <c r="E295" s="14">
         <f t="shared" si="8"/>
-        <v>1.6666666666666666E-2</v>
+        <v>0.36666666666666664</v>
       </c>
       <c r="F295" s="14">
-        <f t="shared" si="8"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="9"/>
+        <v>0.58666666666666656</v>
       </c>
       <c r="G295" s="14">
-        <f t="shared" si="8"/>
-        <v>1.6666666666666666E-2</v>
+        <f t="shared" si="10"/>
+        <v>0.36666666666666664</v>
       </c>
     </row>
     <row r="296" spans="1:7" x14ac:dyDescent="0.3">
@@ -8232,24 +8232,24 @@
         <v>2043</v>
       </c>
       <c r="C296" s="14">
-        <f t="shared" si="8"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="6"/>
+        <v>0.61333333333333317</v>
       </c>
       <c r="D296" s="14">
-        <f t="shared" si="8"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="7"/>
+        <v>0.61333333333333317</v>
       </c>
       <c r="E296" s="14">
         <f t="shared" si="8"/>
-        <v>1.6666666666666666E-2</v>
+        <v>0.3833333333333333</v>
       </c>
       <c r="F296" s="14">
-        <f t="shared" si="8"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="9"/>
+        <v>0.61333333333333317</v>
       </c>
       <c r="G296" s="14">
-        <f t="shared" si="8"/>
-        <v>1.6666666666666666E-2</v>
+        <f t="shared" si="10"/>
+        <v>0.3833333333333333</v>
       </c>
     </row>
     <row r="297" spans="1:7" x14ac:dyDescent="0.3">
@@ -8260,24 +8260,24 @@
         <v>2044</v>
       </c>
       <c r="C297" s="14">
-        <f t="shared" si="8"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="6"/>
+        <v>0.63999999999999979</v>
       </c>
       <c r="D297" s="14">
-        <f t="shared" si="8"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="7"/>
+        <v>0.63999999999999979</v>
       </c>
       <c r="E297" s="14">
         <f t="shared" si="8"/>
-        <v>1.6666666666666666E-2</v>
+        <v>0.39999999999999997</v>
       </c>
       <c r="F297" s="14">
-        <f t="shared" si="8"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="9"/>
+        <v>0.63999999999999979</v>
       </c>
       <c r="G297" s="14">
-        <f t="shared" si="8"/>
-        <v>1.6666666666666666E-2</v>
+        <f t="shared" si="10"/>
+        <v>0.39999999999999997</v>
       </c>
     </row>
     <row r="298" spans="1:7" x14ac:dyDescent="0.3">
@@ -8288,24 +8288,24 @@
         <v>2045</v>
       </c>
       <c r="C298" s="14">
-        <f t="shared" si="8"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="6"/>
+        <v>0.66666666666666641</v>
       </c>
       <c r="D298" s="14">
-        <f t="shared" si="8"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="7"/>
+        <v>0.66666666666666641</v>
       </c>
       <c r="E298" s="14">
         <f t="shared" si="8"/>
-        <v>1.6666666666666666E-2</v>
+        <v>0.41666666666666663</v>
       </c>
       <c r="F298" s="14">
-        <f t="shared" si="8"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="9"/>
+        <v>0.66666666666666641</v>
       </c>
       <c r="G298" s="14">
-        <f t="shared" si="8"/>
-        <v>1.6666666666666666E-2</v>
+        <f t="shared" si="10"/>
+        <v>0.41666666666666663</v>
       </c>
     </row>
     <row r="299" spans="1:7" x14ac:dyDescent="0.3">
@@ -8316,24 +8316,24 @@
         <v>2046</v>
       </c>
       <c r="C299" s="14">
-        <f t="shared" si="8"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="6"/>
+        <v>0.69333333333333302</v>
       </c>
       <c r="D299" s="14">
-        <f t="shared" si="8"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="7"/>
+        <v>0.69333333333333302</v>
       </c>
       <c r="E299" s="14">
         <f t="shared" si="8"/>
-        <v>1.6666666666666666E-2</v>
+        <v>0.43333333333333329</v>
       </c>
       <c r="F299" s="14">
-        <f t="shared" si="8"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="9"/>
+        <v>0.69333333333333302</v>
       </c>
       <c r="G299" s="14">
-        <f t="shared" si="8"/>
-        <v>1.6666666666666666E-2</v>
+        <f t="shared" si="10"/>
+        <v>0.43333333333333329</v>
       </c>
     </row>
     <row r="300" spans="1:7" x14ac:dyDescent="0.3">
@@ -8344,24 +8344,24 @@
         <v>2047</v>
       </c>
       <c r="C300" s="14">
-        <f t="shared" si="8"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="6"/>
+        <v>0.71999999999999964</v>
       </c>
       <c r="D300" s="14">
-        <f t="shared" si="8"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="7"/>
+        <v>0.71999999999999964</v>
       </c>
       <c r="E300" s="14">
         <f t="shared" si="8"/>
-        <v>1.6666666666666666E-2</v>
+        <v>0.44999999999999996</v>
       </c>
       <c r="F300" s="14">
-        <f t="shared" si="8"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="9"/>
+        <v>0.71999999999999964</v>
       </c>
       <c r="G300" s="14">
-        <f t="shared" si="8"/>
-        <v>1.6666666666666666E-2</v>
+        <f t="shared" si="10"/>
+        <v>0.44999999999999996</v>
       </c>
     </row>
     <row r="301" spans="1:7" x14ac:dyDescent="0.3">
@@ -8372,24 +8372,24 @@
         <v>2048</v>
       </c>
       <c r="C301" s="14">
-        <f t="shared" si="8"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="6"/>
+        <v>0.74666666666666626</v>
       </c>
       <c r="D301" s="14">
-        <f t="shared" si="8"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="7"/>
+        <v>0.74666666666666626</v>
       </c>
       <c r="E301" s="14">
         <f t="shared" si="8"/>
-        <v>1.6666666666666666E-2</v>
+        <v>0.46666666666666662</v>
       </c>
       <c r="F301" s="14">
-        <f t="shared" si="8"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="9"/>
+        <v>0.74666666666666626</v>
       </c>
       <c r="G301" s="14">
-        <f t="shared" si="8"/>
-        <v>1.6666666666666666E-2</v>
+        <f t="shared" si="10"/>
+        <v>0.46666666666666662</v>
       </c>
     </row>
     <row r="302" spans="1:7" x14ac:dyDescent="0.3">
@@ -8400,24 +8400,24 @@
         <v>2049</v>
       </c>
       <c r="C302" s="14">
-        <f t="shared" si="8"/>
-        <v>2.6666666666666668E-2</v>
+        <f>C301+(C$303-C$273)/30</f>
+        <v>0.77333333333333287</v>
       </c>
       <c r="D302" s="14">
-        <f t="shared" si="8"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" ref="D302:G302" si="11">D301+(D$303-D$273)/30</f>
+        <v>0.77333333333333287</v>
       </c>
       <c r="E302" s="14">
-        <f t="shared" si="8"/>
-        <v>1.6666666666666666E-2</v>
+        <f t="shared" si="11"/>
+        <v>0.48333333333333328</v>
       </c>
       <c r="F302" s="14">
-        <f t="shared" si="8"/>
-        <v>2.6666666666666668E-2</v>
+        <f t="shared" si="11"/>
+        <v>0.77333333333333287</v>
       </c>
       <c r="G302" s="14">
-        <f t="shared" si="8"/>
-        <v>1.6666666666666666E-2</v>
+        <f t="shared" si="11"/>
+        <v>0.48333333333333328</v>
       </c>
     </row>
     <row r="303" spans="1:7" x14ac:dyDescent="0.3">
@@ -11238,19 +11238,19 @@
         <v>0.05</v>
       </c>
       <c r="D425" s="14">
-        <f t="shared" ref="D425:G433" si="9">D424+(D$434-D$424)/10</f>
+        <f t="shared" ref="D425:G433" si="12">D424+(D$434-D$424)/10</f>
         <v>0.05</v>
       </c>
       <c r="E425" s="14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.05</v>
       </c>
       <c r="F425" s="14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.05</v>
       </c>
       <c r="G425" s="14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.05</v>
       </c>
     </row>
@@ -11262,23 +11262,23 @@
         <v>2022</v>
       </c>
       <c r="C426" s="14">
-        <f t="shared" ref="C426:C433" si="10">C425+(C$434-C$424)/10</f>
+        <f t="shared" ref="C426:C433" si="13">C425+(C$434-C$424)/10</f>
         <v>0.1</v>
       </c>
       <c r="D426" s="14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.1</v>
       </c>
       <c r="E426" s="14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.1</v>
       </c>
       <c r="F426" s="14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.1</v>
       </c>
       <c r="G426" s="14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.1</v>
       </c>
     </row>
@@ -11290,23 +11290,23 @@
         <v>2023</v>
       </c>
       <c r="C427" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.15000000000000002</v>
       </c>
       <c r="D427" s="14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.15000000000000002</v>
       </c>
       <c r="E427" s="14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.15000000000000002</v>
       </c>
       <c r="F427" s="14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.15000000000000002</v>
       </c>
       <c r="G427" s="14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.15000000000000002</v>
       </c>
     </row>
@@ -11318,23 +11318,23 @@
         <v>2024</v>
       </c>
       <c r="C428" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.2</v>
       </c>
       <c r="D428" s="14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.2</v>
       </c>
       <c r="E428" s="14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.2</v>
       </c>
       <c r="F428" s="14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.2</v>
       </c>
       <c r="G428" s="14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.2</v>
       </c>
     </row>
@@ -11346,23 +11346,23 @@
         <v>2025</v>
       </c>
       <c r="C429" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.25</v>
       </c>
       <c r="D429" s="14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.25</v>
       </c>
       <c r="E429" s="14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.25</v>
       </c>
       <c r="F429" s="14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.25</v>
       </c>
       <c r="G429" s="14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.25</v>
       </c>
     </row>
@@ -11374,23 +11374,23 @@
         <v>2026</v>
       </c>
       <c r="C430" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.3</v>
       </c>
       <c r="D430" s="14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.3</v>
       </c>
       <c r="E430" s="14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.3</v>
       </c>
       <c r="F430" s="14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.3</v>
       </c>
       <c r="G430" s="14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.3</v>
       </c>
     </row>
@@ -11402,23 +11402,23 @@
         <v>2027</v>
       </c>
       <c r="C431" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.35</v>
       </c>
       <c r="D431" s="14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.35</v>
       </c>
       <c r="E431" s="14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.35</v>
       </c>
       <c r="F431" s="14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.35</v>
       </c>
       <c r="G431" s="14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.35</v>
       </c>
     </row>
@@ -11430,23 +11430,23 @@
         <v>2028</v>
       </c>
       <c r="C432" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.39999999999999997</v>
       </c>
       <c r="D432" s="14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.39999999999999997</v>
       </c>
       <c r="E432" s="14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.39999999999999997</v>
       </c>
       <c r="F432" s="14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.39999999999999997</v>
       </c>
       <c r="G432" s="14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.39999999999999997</v>
       </c>
     </row>
@@ -11458,23 +11458,23 @@
         <v>2029</v>
       </c>
       <c r="C433" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="D433" s="14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="E433" s="14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="F433" s="14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="G433" s="14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.44999999999999996</v>
       </c>
     </row>
@@ -11513,19 +11513,19 @@
         <v>0.51500000000000001</v>
       </c>
       <c r="D435" s="14">
-        <f t="shared" ref="D435:G435" si="11">D434+(D$454-D$434)/20</f>
+        <f t="shared" ref="D435:G435" si="14">D434+(D$454-D$434)/20</f>
         <v>0.51500000000000001</v>
       </c>
       <c r="E435" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.51500000000000001</v>
       </c>
       <c r="F435" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.51500000000000001</v>
       </c>
       <c r="G435" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.51500000000000001</v>
       </c>
     </row>
@@ -11537,23 +11537,23 @@
         <v>2032</v>
       </c>
       <c r="C436" s="14">
-        <f t="shared" ref="C436:C453" si="12">C435+(C$454-C$434)/20</f>
+        <f t="shared" ref="C436:C453" si="15">C435+(C$454-C$434)/20</f>
         <v>0.53</v>
       </c>
       <c r="D436" s="14">
-        <f t="shared" ref="D436:D453" si="13">D435+(D$454-D$434)/20</f>
+        <f t="shared" ref="D436:D453" si="16">D435+(D$454-D$434)/20</f>
         <v>0.53</v>
       </c>
       <c r="E436" s="14">
-        <f t="shared" ref="E436:E453" si="14">E435+(E$454-E$434)/20</f>
+        <f t="shared" ref="E436:E453" si="17">E435+(E$454-E$434)/20</f>
         <v>0.53</v>
       </c>
       <c r="F436" s="14">
-        <f t="shared" ref="F436:F453" si="15">F435+(F$454-F$434)/20</f>
+        <f t="shared" ref="F436:F453" si="18">F435+(F$454-F$434)/20</f>
         <v>0.53</v>
       </c>
       <c r="G436" s="14">
-        <f t="shared" ref="G436:G453" si="16">G435+(G$454-G$434)/20</f>
+        <f t="shared" ref="G436:G453" si="19">G435+(G$454-G$434)/20</f>
         <v>0.53</v>
       </c>
     </row>
@@ -11565,25 +11565,25 @@
         <v>2033</v>
       </c>
       <c r="C437" s="14">
-        <f t="shared" si="12"/>
-        <v>0.54500000000000004</v>
-      </c>
-      <c r="D437" s="14">
-        <f t="shared" si="13"/>
-        <v>0.54500000000000004</v>
-      </c>
-      <c r="E437" s="14">
-        <f t="shared" si="14"/>
-        <v>0.54500000000000004</v>
-      </c>
-      <c r="F437" s="14">
         <f t="shared" si="15"/>
         <v>0.54500000000000004</v>
       </c>
-      <c r="G437" s="14">
+      <c r="D437" s="14">
         <f t="shared" si="16"/>
         <v>0.54500000000000004</v>
       </c>
+      <c r="E437" s="14">
+        <f t="shared" si="17"/>
+        <v>0.54500000000000004</v>
+      </c>
+      <c r="F437" s="14">
+        <f t="shared" si="18"/>
+        <v>0.54500000000000004</v>
+      </c>
+      <c r="G437" s="14">
+        <f t="shared" si="19"/>
+        <v>0.54500000000000004</v>
+      </c>
     </row>
     <row r="438" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A438" s="1" t="s">
@@ -11593,25 +11593,25 @@
         <v>2034</v>
       </c>
       <c r="C438" s="14">
-        <f t="shared" si="12"/>
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="D438" s="14">
-        <f t="shared" si="13"/>
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="E438" s="14">
-        <f t="shared" si="14"/>
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="F438" s="14">
         <f t="shared" si="15"/>
         <v>0.56000000000000005</v>
       </c>
-      <c r="G438" s="14">
+      <c r="D438" s="14">
         <f t="shared" si="16"/>
         <v>0.56000000000000005</v>
       </c>
+      <c r="E438" s="14">
+        <f t="shared" si="17"/>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="F438" s="14">
+        <f t="shared" si="18"/>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="G438" s="14">
+        <f t="shared" si="19"/>
+        <v>0.56000000000000005</v>
+      </c>
     </row>
     <row r="439" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A439" s="1" t="s">
@@ -11621,25 +11621,25 @@
         <v>2035</v>
       </c>
       <c r="C439" s="14">
-        <f t="shared" si="12"/>
-        <v>0.57500000000000007</v>
-      </c>
-      <c r="D439" s="14">
-        <f t="shared" si="13"/>
-        <v>0.57500000000000007</v>
-      </c>
-      <c r="E439" s="14">
-        <f t="shared" si="14"/>
-        <v>0.57500000000000007</v>
-      </c>
-      <c r="F439" s="14">
         <f t="shared" si="15"/>
         <v>0.57500000000000007</v>
       </c>
-      <c r="G439" s="14">
+      <c r="D439" s="14">
         <f t="shared" si="16"/>
         <v>0.57500000000000007</v>
       </c>
+      <c r="E439" s="14">
+        <f t="shared" si="17"/>
+        <v>0.57500000000000007</v>
+      </c>
+      <c r="F439" s="14">
+        <f t="shared" si="18"/>
+        <v>0.57500000000000007</v>
+      </c>
+      <c r="G439" s="14">
+        <f t="shared" si="19"/>
+        <v>0.57500000000000007</v>
+      </c>
     </row>
     <row r="440" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A440" s="1" t="s">
@@ -11649,25 +11649,25 @@
         <v>2036</v>
       </c>
       <c r="C440" s="14">
-        <f t="shared" si="12"/>
-        <v>0.59000000000000008</v>
-      </c>
-      <c r="D440" s="14">
-        <f t="shared" si="13"/>
-        <v>0.59000000000000008</v>
-      </c>
-      <c r="E440" s="14">
-        <f t="shared" si="14"/>
-        <v>0.59000000000000008</v>
-      </c>
-      <c r="F440" s="14">
         <f t="shared" si="15"/>
         <v>0.59000000000000008</v>
       </c>
-      <c r="G440" s="14">
+      <c r="D440" s="14">
         <f t="shared" si="16"/>
         <v>0.59000000000000008</v>
       </c>
+      <c r="E440" s="14">
+        <f t="shared" si="17"/>
+        <v>0.59000000000000008</v>
+      </c>
+      <c r="F440" s="14">
+        <f t="shared" si="18"/>
+        <v>0.59000000000000008</v>
+      </c>
+      <c r="G440" s="14">
+        <f t="shared" si="19"/>
+        <v>0.59000000000000008</v>
+      </c>
     </row>
     <row r="441" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A441" s="1" t="s">
@@ -11677,25 +11677,25 @@
         <v>2037</v>
       </c>
       <c r="C441" s="14">
-        <f t="shared" si="12"/>
-        <v>0.60500000000000009</v>
-      </c>
-      <c r="D441" s="14">
-        <f t="shared" si="13"/>
-        <v>0.60500000000000009</v>
-      </c>
-      <c r="E441" s="14">
-        <f t="shared" si="14"/>
-        <v>0.60500000000000009</v>
-      </c>
-      <c r="F441" s="14">
         <f t="shared" si="15"/>
         <v>0.60500000000000009</v>
       </c>
-      <c r="G441" s="14">
+      <c r="D441" s="14">
         <f t="shared" si="16"/>
         <v>0.60500000000000009</v>
       </c>
+      <c r="E441" s="14">
+        <f t="shared" si="17"/>
+        <v>0.60500000000000009</v>
+      </c>
+      <c r="F441" s="14">
+        <f t="shared" si="18"/>
+        <v>0.60500000000000009</v>
+      </c>
+      <c r="G441" s="14">
+        <f t="shared" si="19"/>
+        <v>0.60500000000000009</v>
+      </c>
     </row>
     <row r="442" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A442" s="1" t="s">
@@ -11705,25 +11705,25 @@
         <v>2038</v>
       </c>
       <c r="C442" s="14">
-        <f t="shared" si="12"/>
-        <v>0.62000000000000011</v>
-      </c>
-      <c r="D442" s="14">
-        <f t="shared" si="13"/>
-        <v>0.62000000000000011</v>
-      </c>
-      <c r="E442" s="14">
-        <f t="shared" si="14"/>
-        <v>0.62000000000000011</v>
-      </c>
-      <c r="F442" s="14">
         <f t="shared" si="15"/>
         <v>0.62000000000000011</v>
       </c>
-      <c r="G442" s="14">
+      <c r="D442" s="14">
         <f t="shared" si="16"/>
         <v>0.62000000000000011</v>
       </c>
+      <c r="E442" s="14">
+        <f t="shared" si="17"/>
+        <v>0.62000000000000011</v>
+      </c>
+      <c r="F442" s="14">
+        <f t="shared" si="18"/>
+        <v>0.62000000000000011</v>
+      </c>
+      <c r="G442" s="14">
+        <f t="shared" si="19"/>
+        <v>0.62000000000000011</v>
+      </c>
     </row>
     <row r="443" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A443" s="1" t="s">
@@ -11733,25 +11733,25 @@
         <v>2039</v>
       </c>
       <c r="C443" s="14">
-        <f t="shared" si="12"/>
-        <v>0.63500000000000012</v>
-      </c>
-      <c r="D443" s="14">
-        <f t="shared" si="13"/>
-        <v>0.63500000000000012</v>
-      </c>
-      <c r="E443" s="14">
-        <f t="shared" si="14"/>
-        <v>0.63500000000000012</v>
-      </c>
-      <c r="F443" s="14">
         <f t="shared" si="15"/>
         <v>0.63500000000000012</v>
       </c>
-      <c r="G443" s="14">
+      <c r="D443" s="14">
         <f t="shared" si="16"/>
         <v>0.63500000000000012</v>
       </c>
+      <c r="E443" s="14">
+        <f t="shared" si="17"/>
+        <v>0.63500000000000012</v>
+      </c>
+      <c r="F443" s="14">
+        <f t="shared" si="18"/>
+        <v>0.63500000000000012</v>
+      </c>
+      <c r="G443" s="14">
+        <f t="shared" si="19"/>
+        <v>0.63500000000000012</v>
+      </c>
     </row>
     <row r="444" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A444" s="1" t="s">
@@ -11761,25 +11761,25 @@
         <v>2040</v>
       </c>
       <c r="C444" s="14">
-        <f t="shared" si="12"/>
-        <v>0.65000000000000013</v>
-      </c>
-      <c r="D444" s="14">
-        <f t="shared" si="13"/>
-        <v>0.65000000000000013</v>
-      </c>
-      <c r="E444" s="14">
-        <f t="shared" si="14"/>
-        <v>0.65000000000000013</v>
-      </c>
-      <c r="F444" s="14">
         <f t="shared" si="15"/>
         <v>0.65000000000000013</v>
       </c>
-      <c r="G444" s="14">
+      <c r="D444" s="14">
         <f t="shared" si="16"/>
         <v>0.65000000000000013</v>
       </c>
+      <c r="E444" s="14">
+        <f t="shared" si="17"/>
+        <v>0.65000000000000013</v>
+      </c>
+      <c r="F444" s="14">
+        <f t="shared" si="18"/>
+        <v>0.65000000000000013</v>
+      </c>
+      <c r="G444" s="14">
+        <f t="shared" si="19"/>
+        <v>0.65000000000000013</v>
+      </c>
     </row>
     <row r="445" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A445" s="1" t="s">
@@ -11789,25 +11789,25 @@
         <v>2041</v>
       </c>
       <c r="C445" s="14">
-        <f t="shared" si="12"/>
-        <v>0.66500000000000015</v>
-      </c>
-      <c r="D445" s="14">
-        <f t="shared" si="13"/>
-        <v>0.66500000000000015</v>
-      </c>
-      <c r="E445" s="14">
-        <f t="shared" si="14"/>
-        <v>0.66500000000000015</v>
-      </c>
-      <c r="F445" s="14">
         <f t="shared" si="15"/>
         <v>0.66500000000000015</v>
       </c>
-      <c r="G445" s="14">
+      <c r="D445" s="14">
         <f t="shared" si="16"/>
         <v>0.66500000000000015</v>
       </c>
+      <c r="E445" s="14">
+        <f t="shared" si="17"/>
+        <v>0.66500000000000015</v>
+      </c>
+      <c r="F445" s="14">
+        <f t="shared" si="18"/>
+        <v>0.66500000000000015</v>
+      </c>
+      <c r="G445" s="14">
+        <f t="shared" si="19"/>
+        <v>0.66500000000000015</v>
+      </c>
     </row>
     <row r="446" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A446" s="1" t="s">
@@ -11817,25 +11817,25 @@
         <v>2042</v>
       </c>
       <c r="C446" s="14">
-        <f t="shared" si="12"/>
-        <v>0.68000000000000016</v>
-      </c>
-      <c r="D446" s="14">
-        <f t="shared" si="13"/>
-        <v>0.68000000000000016</v>
-      </c>
-      <c r="E446" s="14">
-        <f t="shared" si="14"/>
-        <v>0.68000000000000016</v>
-      </c>
-      <c r="F446" s="14">
         <f t="shared" si="15"/>
         <v>0.68000000000000016</v>
       </c>
-      <c r="G446" s="14">
+      <c r="D446" s="14">
         <f t="shared" si="16"/>
         <v>0.68000000000000016</v>
       </c>
+      <c r="E446" s="14">
+        <f t="shared" si="17"/>
+        <v>0.68000000000000016</v>
+      </c>
+      <c r="F446" s="14">
+        <f t="shared" si="18"/>
+        <v>0.68000000000000016</v>
+      </c>
+      <c r="G446" s="14">
+        <f t="shared" si="19"/>
+        <v>0.68000000000000016</v>
+      </c>
     </row>
     <row r="447" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A447" s="1" t="s">
@@ -11845,25 +11845,25 @@
         <v>2043</v>
       </c>
       <c r="C447" s="14">
-        <f t="shared" si="12"/>
-        <v>0.69500000000000017</v>
-      </c>
-      <c r="D447" s="14">
-        <f t="shared" si="13"/>
-        <v>0.69500000000000017</v>
-      </c>
-      <c r="E447" s="14">
-        <f t="shared" si="14"/>
-        <v>0.69500000000000017</v>
-      </c>
-      <c r="F447" s="14">
         <f t="shared" si="15"/>
         <v>0.69500000000000017</v>
       </c>
-      <c r="G447" s="14">
+      <c r="D447" s="14">
         <f t="shared" si="16"/>
         <v>0.69500000000000017</v>
       </c>
+      <c r="E447" s="14">
+        <f t="shared" si="17"/>
+        <v>0.69500000000000017</v>
+      </c>
+      <c r="F447" s="14">
+        <f t="shared" si="18"/>
+        <v>0.69500000000000017</v>
+      </c>
+      <c r="G447" s="14">
+        <f t="shared" si="19"/>
+        <v>0.69500000000000017</v>
+      </c>
     </row>
     <row r="448" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A448" s="1" t="s">
@@ -11873,25 +11873,25 @@
         <v>2044</v>
       </c>
       <c r="C448" s="14">
-        <f t="shared" si="12"/>
-        <v>0.71000000000000019</v>
-      </c>
-      <c r="D448" s="14">
-        <f t="shared" si="13"/>
-        <v>0.71000000000000019</v>
-      </c>
-      <c r="E448" s="14">
-        <f t="shared" si="14"/>
-        <v>0.71000000000000019</v>
-      </c>
-      <c r="F448" s="14">
         <f t="shared" si="15"/>
         <v>0.71000000000000019</v>
       </c>
-      <c r="G448" s="14">
+      <c r="D448" s="14">
         <f t="shared" si="16"/>
         <v>0.71000000000000019</v>
       </c>
+      <c r="E448" s="14">
+        <f t="shared" si="17"/>
+        <v>0.71000000000000019</v>
+      </c>
+      <c r="F448" s="14">
+        <f t="shared" si="18"/>
+        <v>0.71000000000000019</v>
+      </c>
+      <c r="G448" s="14">
+        <f t="shared" si="19"/>
+        <v>0.71000000000000019</v>
+      </c>
     </row>
     <row r="449" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A449" s="1" t="s">
@@ -11901,25 +11901,25 @@
         <v>2045</v>
       </c>
       <c r="C449" s="14">
-        <f t="shared" si="12"/>
-        <v>0.7250000000000002</v>
-      </c>
-      <c r="D449" s="14">
-        <f t="shared" si="13"/>
-        <v>0.7250000000000002</v>
-      </c>
-      <c r="E449" s="14">
-        <f t="shared" si="14"/>
-        <v>0.7250000000000002</v>
-      </c>
-      <c r="F449" s="14">
         <f t="shared" si="15"/>
         <v>0.7250000000000002</v>
       </c>
-      <c r="G449" s="14">
+      <c r="D449" s="14">
         <f t="shared" si="16"/>
         <v>0.7250000000000002</v>
       </c>
+      <c r="E449" s="14">
+        <f t="shared" si="17"/>
+        <v>0.7250000000000002</v>
+      </c>
+      <c r="F449" s="14">
+        <f t="shared" si="18"/>
+        <v>0.7250000000000002</v>
+      </c>
+      <c r="G449" s="14">
+        <f t="shared" si="19"/>
+        <v>0.7250000000000002</v>
+      </c>
     </row>
     <row r="450" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A450" s="1" t="s">
@@ -11929,25 +11929,25 @@
         <v>2046</v>
       </c>
       <c r="C450" s="14">
-        <f t="shared" si="12"/>
-        <v>0.74000000000000021</v>
-      </c>
-      <c r="D450" s="14">
-        <f t="shared" si="13"/>
-        <v>0.74000000000000021</v>
-      </c>
-      <c r="E450" s="14">
-        <f t="shared" si="14"/>
-        <v>0.74000000000000021</v>
-      </c>
-      <c r="F450" s="14">
         <f t="shared" si="15"/>
         <v>0.74000000000000021</v>
       </c>
-      <c r="G450" s="14">
+      <c r="D450" s="14">
         <f t="shared" si="16"/>
         <v>0.74000000000000021</v>
       </c>
+      <c r="E450" s="14">
+        <f t="shared" si="17"/>
+        <v>0.74000000000000021</v>
+      </c>
+      <c r="F450" s="14">
+        <f t="shared" si="18"/>
+        <v>0.74000000000000021</v>
+      </c>
+      <c r="G450" s="14">
+        <f t="shared" si="19"/>
+        <v>0.74000000000000021</v>
+      </c>
     </row>
     <row r="451" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A451" s="1" t="s">
@@ -11957,25 +11957,25 @@
         <v>2047</v>
       </c>
       <c r="C451" s="14">
-        <f t="shared" si="12"/>
-        <v>0.75500000000000023</v>
-      </c>
-      <c r="D451" s="14">
-        <f t="shared" si="13"/>
-        <v>0.75500000000000023</v>
-      </c>
-      <c r="E451" s="14">
-        <f t="shared" si="14"/>
-        <v>0.75500000000000023</v>
-      </c>
-      <c r="F451" s="14">
         <f t="shared" si="15"/>
         <v>0.75500000000000023</v>
       </c>
-      <c r="G451" s="14">
+      <c r="D451" s="14">
         <f t="shared" si="16"/>
         <v>0.75500000000000023</v>
       </c>
+      <c r="E451" s="14">
+        <f t="shared" si="17"/>
+        <v>0.75500000000000023</v>
+      </c>
+      <c r="F451" s="14">
+        <f t="shared" si="18"/>
+        <v>0.75500000000000023</v>
+      </c>
+      <c r="G451" s="14">
+        <f t="shared" si="19"/>
+        <v>0.75500000000000023</v>
+      </c>
     </row>
     <row r="452" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A452" s="1" t="s">
@@ -11985,25 +11985,25 @@
         <v>2048</v>
       </c>
       <c r="C452" s="14">
-        <f t="shared" si="12"/>
-        <v>0.77000000000000024</v>
-      </c>
-      <c r="D452" s="14">
-        <f t="shared" si="13"/>
-        <v>0.77000000000000024</v>
-      </c>
-      <c r="E452" s="14">
-        <f t="shared" si="14"/>
-        <v>0.77000000000000024</v>
-      </c>
-      <c r="F452" s="14">
         <f t="shared" si="15"/>
         <v>0.77000000000000024</v>
       </c>
-      <c r="G452" s="14">
+      <c r="D452" s="14">
         <f t="shared" si="16"/>
         <v>0.77000000000000024</v>
       </c>
+      <c r="E452" s="14">
+        <f t="shared" si="17"/>
+        <v>0.77000000000000024</v>
+      </c>
+      <c r="F452" s="14">
+        <f t="shared" si="18"/>
+        <v>0.77000000000000024</v>
+      </c>
+      <c r="G452" s="14">
+        <f t="shared" si="19"/>
+        <v>0.77000000000000024</v>
+      </c>
     </row>
     <row r="453" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A453" s="1" t="s">
@@ -12013,23 +12013,23 @@
         <v>2049</v>
       </c>
       <c r="C453" s="14">
-        <f t="shared" si="12"/>
-        <v>0.78500000000000025</v>
-      </c>
-      <c r="D453" s="14">
-        <f t="shared" si="13"/>
-        <v>0.78500000000000025</v>
-      </c>
-      <c r="E453" s="14">
-        <f t="shared" si="14"/>
-        <v>0.78500000000000025</v>
-      </c>
-      <c r="F453" s="14">
         <f t="shared" si="15"/>
         <v>0.78500000000000025</v>
       </c>
+      <c r="D453" s="14">
+        <f t="shared" si="16"/>
+        <v>0.78500000000000025</v>
+      </c>
+      <c r="E453" s="14">
+        <f t="shared" si="17"/>
+        <v>0.78500000000000025</v>
+      </c>
+      <c r="F453" s="14">
+        <f t="shared" si="18"/>
+        <v>0.78500000000000025</v>
+      </c>
       <c r="G453" s="14">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0.78500000000000025</v>
       </c>
     </row>

</xml_diff>